<commit_message>
Start $ERJ update model
</commit_message>
<xml_diff>
--- a/$SPOT.xlsx
+++ b/$SPOT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849F58DF-B815-4C7B-B779-92634D463ECF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07CCB2-2D0F-423C-965D-E4D24425D6C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1635" yWindow="1260" windowWidth="27165" windowHeight="14100" activeTab="1" xr2:uid="{1B36FFFD-D458-4A57-865C-CCAC07CF1B21}"/>
   </bookViews>
@@ -738,6 +738,28 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,33 +772,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1257,24 +1257,24 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="G5" s="45" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="G5" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="47"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="46"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="D8" s="15"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="43" t="s">
         <v>138</v>
       </c>
       <c r="I8" s="6"/>
@@ -1471,11 +1471,11 @@
       <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
       <c r="G15" s="13"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1495,10 +1495,10 @@
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="D16" s="42"/>
+      <c r="D16" s="50"/>
       <c r="G16" s="13"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1515,10 +1515,10 @@
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="42"/>
+      <c r="D17" s="50"/>
       <c r="G17" s="13"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1535,10 +1535,10 @@
       <c r="B18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="42"/>
+      <c r="D18" s="50"/>
       <c r="G18" s="13"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1558,10 +1558,10 @@
       <c r="B19" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="44"/>
+      <c r="D19" s="52"/>
       <c r="G19" s="13"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1601,11 +1601,11 @@
       <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="46"/>
       <c r="G22" s="13"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1622,10 +1622,10 @@
       <c r="B23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="42"/>
+      <c r="D23" s="50"/>
       <c r="G23" s="13"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1642,10 +1642,10 @@
       <c r="B24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="53">
         <v>2006</v>
       </c>
-      <c r="D24" s="42"/>
+      <c r="D24" s="50"/>
       <c r="G24" s="13"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1662,10 +1662,10 @@
       <c r="B25" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="53">
         <v>2018</v>
       </c>
-      <c r="D25" s="42"/>
+      <c r="D25" s="50"/>
       <c r="G25" s="13"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1680,8 +1680,8 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="42"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="50"/>
       <c r="G26" s="13"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1698,11 +1698,11 @@
       <c r="B27" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="53">
         <f>+'Financial Model'!Q30</f>
         <v>640</v>
       </c>
-      <c r="D27" s="42"/>
+      <c r="D27" s="50"/>
       <c r="G27" s="13"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -1719,11 +1719,11 @@
       <c r="B28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="54">
         <f>+'Financial Model'!AA42</f>
         <v>9123</v>
       </c>
-      <c r="D28" s="42"/>
+      <c r="D28" s="50"/>
       <c r="G28" s="13"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -1738,8 +1738,8 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" s="13"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="42"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="50"/>
       <c r="G29" s="13"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -1779,8 +1779,8 @@
       <c r="B31" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
       <c r="G31" s="14"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -1794,31 +1794,31 @@
       <c r="Q31" s="10"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="47"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="46"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="47">
         <f>C6/('Financial Model'!Q19*[1]Currencies!$C$4)</f>
         <v>2.048085692097604</v>
       </c>
-      <c r="D35" s="51"/>
+      <c r="D35" s="48"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="50">
+      <c r="C36" s="47">
         <f>C8/(SUM('Financial Model'!N8:Q8)*[1]Currencies!$C$4)</f>
         <v>19.19263634517079</v>
       </c>
-      <c r="D36" s="51"/>
+      <c r="D36" s="48"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="13" t="s">
@@ -1831,11 +1831,11 @@
       <c r="B38" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="50">
+      <c r="C38" s="47">
         <f>C6/(SUM('Financial Model'!N18:Q18)*[1]Currencies!$C$4)</f>
         <v>118.16107002434873</v>
       </c>
-      <c r="D38" s="51"/>
+      <c r="D38" s="48"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="13" t="s">
@@ -1848,19 +1848,14 @@
       <c r="B40" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="50">
+      <c r="C40" s="47">
         <f>C6/('Financial Model'!Q100*[1]Currencies!$C$4)</f>
         <v>117.04538845662525</v>
       </c>
-      <c r="D40" s="51"/>
+      <c r="D40" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="G5:Q5"/>
@@ -1877,6 +1872,11 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1891,7 +1891,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1947,7 +1947,7 @@
       <c r="P1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="28" t="s">
         <v>30</v>
       </c>
       <c r="R1" s="21" t="s">
@@ -2072,7 +2072,7 @@
       <c r="P3" s="24">
         <v>45474</v>
       </c>
-      <c r="Q3" s="52">
+      <c r="Q3" s="41">
         <v>45608</v>
       </c>
       <c r="AA3" s="32">
@@ -4130,6 +4130,9 @@
       <c r="N46" s="17">
         <v>300</v>
       </c>
+      <c r="O46" s="17">
+        <v>274</v>
+      </c>
       <c r="P46" s="17">
         <v>254</v>
       </c>
@@ -4144,6 +4147,9 @@
       <c r="N47" s="17">
         <v>247</v>
       </c>
+      <c r="O47" s="17">
+        <v>224</v>
+      </c>
       <c r="P47" s="17">
         <v>211</v>
       </c>
@@ -4159,6 +4165,10 @@
         <f>1137+84</f>
         <v>1221</v>
       </c>
+      <c r="O48" s="17">
+        <f>1159+76</f>
+        <v>1235</v>
+      </c>
       <c r="P48" s="17">
         <f>1167+68</f>
         <v>1235</v>
@@ -4175,6 +4185,9 @@
       <c r="N49" s="26">
         <v>1215</v>
       </c>
+      <c r="O49" s="26">
+        <v>1534</v>
+      </c>
       <c r="P49" s="26">
         <v>1931</v>
       </c>
@@ -4189,6 +4202,9 @@
       <c r="N50" s="17">
         <v>75</v>
       </c>
+      <c r="O50" s="17">
+        <v>72</v>
+      </c>
       <c r="P50" s="17">
         <v>70</v>
       </c>
@@ -4203,6 +4219,9 @@
       <c r="N51" s="17">
         <v>0</v>
       </c>
+      <c r="O51" s="17">
+        <v>51</v>
+      </c>
       <c r="P51" s="17">
         <v>52</v>
       </c>
@@ -4217,6 +4236,9 @@
       <c r="N52" s="17">
         <v>28</v>
       </c>
+      <c r="O52" s="17">
+        <v>41</v>
+      </c>
       <c r="P52" s="17">
         <v>49</v>
       </c>
@@ -4231,6 +4253,9 @@
       <c r="N53" s="17">
         <v>858</v>
       </c>
+      <c r="O53" s="17">
+        <v>777</v>
+      </c>
       <c r="P53" s="17">
         <v>753</v>
       </c>
@@ -4245,6 +4270,9 @@
       <c r="N54" s="17">
         <v>20</v>
       </c>
+      <c r="O54" s="17">
+        <v>21</v>
+      </c>
       <c r="P54" s="17">
         <v>35</v>
       </c>
@@ -4259,6 +4287,9 @@
       <c r="N55" s="26">
         <v>1100</v>
       </c>
+      <c r="O55" s="26">
+        <v>1220</v>
+      </c>
       <c r="P55" s="26">
         <v>1344</v>
       </c>
@@ -4273,6 +4304,9 @@
       <c r="N56" s="26">
         <v>3114</v>
       </c>
+      <c r="O56" s="26">
+        <v>3451</v>
+      </c>
       <c r="P56" s="26">
         <v>4054</v>
       </c>
@@ -4287,6 +4321,9 @@
       <c r="N57" s="17">
         <v>168</v>
       </c>
+      <c r="O57" s="17">
+        <v>175</v>
+      </c>
       <c r="P57" s="17">
         <v>158</v>
       </c>
@@ -4301,6 +4338,10 @@
       <c r="N58" s="17">
         <f>SUM(N46:N57)</f>
         <v>8346</v>
+      </c>
+      <c r="O58" s="17">
+        <f>SUM(O46:O57)</f>
+        <v>9075</v>
       </c>
       <c r="P58" s="17">
         <f>SUM(P46:P57)</f>
@@ -4319,6 +4360,9 @@
       <c r="N60" s="26">
         <v>1203</v>
       </c>
+      <c r="O60" s="26">
+        <v>1270</v>
+      </c>
       <c r="P60" s="26">
         <v>1323</v>
       </c>
@@ -4333,6 +4377,9 @@
       <c r="N61" s="17">
         <v>493</v>
       </c>
+      <c r="O61" s="17">
+        <v>493</v>
+      </c>
       <c r="P61" s="17">
         <v>472</v>
       </c>
@@ -4347,6 +4394,9 @@
       <c r="N62" s="17">
         <v>26</v>
       </c>
+      <c r="O62" s="17">
+        <v>17</v>
+      </c>
       <c r="P62" s="17">
         <v>11</v>
       </c>
@@ -4361,6 +4411,9 @@
       <c r="N63" s="17">
         <v>3</v>
       </c>
+      <c r="O63" s="17">
+        <v>3</v>
+      </c>
       <c r="P63" s="17">
         <v>3</v>
       </c>
@@ -4375,6 +4428,9 @@
       <c r="N64" s="17">
         <v>8</v>
       </c>
+      <c r="O64" s="17">
+        <v>17</v>
+      </c>
       <c r="P64" s="17">
         <v>19</v>
       </c>
@@ -4389,6 +4445,9 @@
       <c r="N65" s="17">
         <v>978</v>
       </c>
+      <c r="O65" s="17">
+        <v>1048</v>
+      </c>
       <c r="P65" s="17">
         <v>1091</v>
       </c>
@@ -4403,6 +4462,9 @@
       <c r="N66" s="17">
         <v>12</v>
       </c>
+      <c r="O66" s="17">
+        <v>14</v>
+      </c>
       <c r="P66" s="17">
         <v>17</v>
       </c>
@@ -4417,6 +4479,9 @@
       <c r="N67" s="17">
         <v>622</v>
       </c>
+      <c r="O67" s="17">
+        <v>634</v>
+      </c>
       <c r="P67" s="17">
         <v>657</v>
       </c>
@@ -4431,6 +4496,9 @@
       <c r="N68" s="17">
         <v>2440</v>
       </c>
+      <c r="O68" s="17">
+        <v>2228</v>
+      </c>
       <c r="P68" s="17">
         <v>2223</v>
       </c>
@@ -4445,6 +4513,9 @@
       <c r="N69" s="17">
         <v>21</v>
       </c>
+      <c r="O69" s="17">
+        <v>20</v>
+      </c>
       <c r="P69" s="17">
         <v>24</v>
       </c>
@@ -4459,6 +4530,9 @@
       <c r="N70" s="26">
         <v>17</v>
       </c>
+      <c r="O70" s="26">
+        <v>22</v>
+      </c>
       <c r="P70" s="26">
         <v>47</v>
       </c>
@@ -4473,6 +4547,10 @@
       <c r="N71" s="17">
         <f>SUM(N60:N70)</f>
         <v>5823</v>
+      </c>
+      <c r="O71" s="17">
+        <f>SUM(O60:O70)</f>
+        <v>5766</v>
       </c>
       <c r="P71" s="17">
         <f>SUM(P60:P70)</f>
@@ -4491,6 +4569,9 @@
       <c r="N73" s="17">
         <v>2523</v>
       </c>
+      <c r="O73" s="17">
+        <v>3309</v>
+      </c>
       <c r="P73" s="17">
         <v>4259</v>
       </c>
@@ -4506,6 +4587,10 @@
         <f>N73+N71</f>
         <v>8346</v>
       </c>
+      <c r="O74" s="17">
+        <f>O73+O71</f>
+        <v>9075</v>
+      </c>
       <c r="P74" s="17">
         <f>P73+P71</f>
         <v>10146</v>
@@ -4520,6 +4605,10 @@
         <v>74</v>
       </c>
       <c r="N76" s="17"/>
+      <c r="O76" s="17">
+        <f>O58-O71</f>
+        <v>3309</v>
+      </c>
       <c r="P76" s="17">
         <f>P58-P71</f>
         <v>4259</v>
@@ -4533,6 +4622,10 @@
       <c r="B77" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="O77" s="1">
+        <f>O76/O19</f>
+        <v>16.709972883486252</v>
+      </c>
       <c r="P77" s="1">
         <f>P76/P19</f>
         <v>21.299348048910705</v>
@@ -4550,6 +4643,10 @@
         <f>+N49+N55+N56</f>
         <v>5429</v>
       </c>
+      <c r="O79" s="17">
+        <f>+O49+O55+O56</f>
+        <v>6205</v>
+      </c>
       <c r="P79" s="17">
         <f>+P49+P55+P56</f>
         <v>7329</v>
@@ -4567,6 +4664,10 @@
         <f>+N60+N70</f>
         <v>1220</v>
       </c>
+      <c r="O80" s="17">
+        <f>+O60+O70</f>
+        <v>1292</v>
+      </c>
       <c r="P80" s="17">
         <f>+P60+P70</f>
         <v>1370</v>
@@ -4584,6 +4685,10 @@
         <f>N79-N80</f>
         <v>4209</v>
       </c>
+      <c r="O81" s="17">
+        <f>O79-O80</f>
+        <v>4913</v>
+      </c>
       <c r="P81" s="17">
         <f>P79-P80</f>
         <v>5959</v>
@@ -4641,15 +4746,19 @@
         <v>136</v>
       </c>
     </row>
-    <row r="88" spans="2:27" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="53" t="s">
+    <row r="88" spans="2:27" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="P88" s="53">
+      <c r="O88" s="42">
+        <f>+O83/O77</f>
+        <v>15.79296398863705</v>
+      </c>
+      <c r="P88" s="42">
         <f>+P83/P77</f>
         <v>14.73237581166471</v>
       </c>
-      <c r="Q88" s="53">
+      <c r="Q88" s="42">
         <f>+Q83/Q77</f>
         <v>16.03424219189294</v>
       </c>
@@ -4850,13 +4959,14 @@
     <hyperlink ref="H1" r:id="rId6" xr:uid="{D41EEB08-11F5-44A0-AE7C-6D2A90771DA1}"/>
     <hyperlink ref="G1" r:id="rId7" xr:uid="{B826FA8F-1C74-496D-8D94-CD8D3D7C295B}"/>
     <hyperlink ref="E1" r:id="rId8" xr:uid="{8F38F335-CB1A-4AF1-82E9-A4C1724F4702}"/>
+    <hyperlink ref="Q1" r:id="rId9" xr:uid="{ABB2003F-1E0D-4DE3-B941-A1C9955BCB3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId10"/>
   <ignoredErrors>
     <ignoredError sqref="N8:N17 J6:J8 J12 J15 J17 N31:N36 F8:F19 J31:J35" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>